<commit_message>
Python modules and datasets
</commit_message>
<xml_diff>
--- a/vishal/datasets/production_plans.xlsx
+++ b/vishal/datasets/production_plans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vishal\PycharmProjects\mindshift\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C655DA-DD3A-448B-9EFE-BB701E8DC22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0080FE-F862-4727-BB0A-8C5D235D8590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="21">
   <si>
     <t>plan_id</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>PLN-002</t>
-  </si>
-  <si>
-    <t>2024-04-21 16:34:34.196712</t>
   </si>
 </sst>
 </file>
@@ -454,15 +451,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:K30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.21875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -504,7 +499,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="2">
-        <v>45403.689928448679</v>
+        <v>45403.689928449072</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -539,7 +534,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="2">
-        <v>45403.689928448679</v>
+        <v>45403.689928449072</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -574,7 +569,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>45403.689928448679</v>
+        <v>45403.689928449072</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -609,7 +604,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2">
-        <v>45403.689928448679</v>
+        <v>45403.689928449072</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -644,7 +639,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2">
-        <v>45403.689928448679</v>
+        <v>45403.689928449072</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -679,7 +674,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="2">
-        <v>45403.689928448679</v>
+        <v>45403.689928449072</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -714,7 +709,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>45403.689928448679</v>
+        <v>45403.689928449072</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -749,7 +744,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>45403.689928448679</v>
+        <v>45403.689928449072</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -784,7 +779,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2">
-        <v>45403.689928448679</v>
+        <v>45403.689928449072</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -818,8 +813,8 @@
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
-        <v>21</v>
+      <c r="B11" s="2">
+        <v>45403.690673573059</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -853,8 +848,8 @@
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
-        <v>21</v>
+      <c r="B12" s="2">
+        <v>45403.690673573059</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -888,8 +883,8 @@
       <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
-        <v>21</v>
+      <c r="B13" s="2">
+        <v>45403.690673573059</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -923,8 +918,8 @@
       <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
-        <v>21</v>
+      <c r="B14" s="2">
+        <v>45403.690673573059</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -958,8 +953,8 @@
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
-        <v>21</v>
+      <c r="B15" s="2">
+        <v>45403.690673573059</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
@@ -993,8 +988,8 @@
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" t="s">
-        <v>21</v>
+      <c r="B16" s="2">
+        <v>45403.690673573059</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
@@ -1028,8 +1023,8 @@
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" t="s">
-        <v>21</v>
+      <c r="B17" s="2">
+        <v>45403.690673573059</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -1063,8 +1058,8 @@
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
-        <v>21</v>
+      <c r="B18" s="2">
+        <v>45403.690673573059</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -1098,8 +1093,8 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
-        <v>21</v>
+      <c r="B19" s="2">
+        <v>45403.690673573059</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -1128,6 +1123,61 @@
       <c r="K19" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D20" s="3"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D21" s="3"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D22" s="3"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D23" s="3"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D24" s="3"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D25" s="3"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D26" s="3"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D27" s="3"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D28" s="3"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D29" s="3"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D30" s="3"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>